<commit_message>
Tijden van wbs aangepast
</commit_message>
<xml_diff>
--- a/Workbreakdownstructure.xlsx
+++ b/Workbreakdownstructure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rocteraa365-my.sharepoint.com/personal/77013_rocteraa-student_nl/Documents/proftaak/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proftaak\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t>WBS id</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <dimension ref="A1:J1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -593,7 +596,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -615,7 +618,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -635,7 +638,7 @@
         <v>17</v>
       </c>
       <c r="G7" s="2">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -658,7 +661,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -681,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -727,7 +730,7 @@
         <v>22</v>
       </c>
       <c r="G11" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -750,7 +753,7 @@
         <v>22</v>
       </c>
       <c r="G12" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -773,7 +776,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -796,7 +799,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="G15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -840,7 +843,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -862,7 +865,9 @@
       <c r="F17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -884,7 +889,7 @@
         <v>38</v>
       </c>
       <c r="G18" s="2">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -910,12 +915,10 @@
       </c>
       <c r="E21" s="3"/>
       <c r="G21" s="2">
-        <f>SUBTOTAL(9,G5:G18)</f>
-        <v>38</v>
-      </c>
-      <c r="H21" s="1">
-        <f>SUBTOTAL(9,H7)</f>
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
plan van aanpak in het projectplan gezet
</commit_message>
<xml_diff>
--- a/Workbreakdownstructure.xlsx
+++ b/Workbreakdownstructure.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A1:J1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
         <v>17</v>
       </c>
       <c r="G7" s="2">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="G9" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="2">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>22</v>
       </c>
       <c r="G11" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>22</v>
       </c>
       <c r="G12" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>22</v>
       </c>
       <c r="G13" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="G15" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -915,7 +915,8 @@
       </c>
       <c r="E21" s="3"/>
       <c r="G21" s="2">
-        <v>117</v>
+        <f>SUM(G5:G18)</f>
+        <v>198</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>42</v>

</xml_diff>